<commit_message>
[chore] Rename recipe-swr with uppercase
</commit_message>
<xml_diff>
--- a/SWR.xlsx
+++ b/SWR.xlsx
@@ -78,7 +78,7 @@
     <t>DESIGNATOR</t>
   </si>
   <si>
-    <t>123456-ExtraPlace</t>
+    <t>123456-EXTRAPLACE</t>
   </si>
   <si>
     <t>590-123456</t>
@@ -102,7 +102,7 @@
 J1000</t>
   </si>
   <si>
-    <t>123457-NoPlace-ALL</t>
+    <t>123457-NOPLACE-ALL</t>
   </si>
   <si>
     <t>NO PLACE
@@ -120,7 +120,7 @@
 J3</t>
   </si>
   <si>
-    <t>123458-NoPlace-Partial</t>
+    <t>123458-NOPLACE-PARTIAL</t>
   </si>
   <si>
     <t>NO PLACE</t>
@@ -132,7 +132,7 @@
     <t>R107,R112-R113</t>
   </si>
   <si>
-    <t>123459-PartSub-ALL</t>
+    <t>123459-PARTSUB-ALL</t>
   </si>
   <si>
     <t>510-500956A
@@ -140,7 +140,7 @@
 531-500480A</t>
   </si>
   <si>
-    <t>123460-PartSub-Partial</t>
+    <t>123460-PARTSUB-PARTIAL</t>
   </si>
   <si>
     <t>510-500956A</t>
@@ -321,12 +321,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1151,17 +1151,13 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.4444444444444" customWidth="1"/>
     <col min="2" max="2" width="11.8888888888889" customWidth="1"/>
@@ -1203,7 +1199,7 @@
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:9">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1226,7 +1222,7 @@
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:9">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1249,7 +1245,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1272,7 +1268,7 @@
       </c>
     </row>
     <row r="5" ht="43.2" spans="1:9">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1295,7 +1291,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1317,8 +1313,32 @@
         <v>29</v>
       </c>
     </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="str">
+        <f>UPPER(A8)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="str">
+        <f>UPPER(A9)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" t="str">
+        <f>UPPER(A10)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" t="str">
+        <f>UPPER(A11)</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A$1:A$1048576">
+  <conditionalFormatting sqref="A1 A7:A1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1336,9 +1356,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>

</xml_diff>